<commit_message>
Complete implementation and unit testing
Signed-off-by: Gary O'Neall <gary@sourceauditor.com>
</commit_message>
<xml_diff>
--- a/spdx-spreadsheet-store/TestFiles/SPDXSpreadsheetExample-v2.2.xlsx
+++ b/spdx-spreadsheet-store/TestFiles/SPDXSpreadsheetExample-v2.2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gary\git\Spdx-Java-Spreadsheet-Store\spdx-spreadsheet-store\TestFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F92327F-DDEE-4CBF-B47E-DF4848116421}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B834D6BF-6116-487B-8656-A5279261A2D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="209">
   <si>
     <t>Spreadsheet Version</t>
   </si>
@@ -827,7 +827,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -838,6 +838,11 @@
       <patternFill patternType="solid">
         <fgColor indexed="22"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="22"/>
       </patternFill>
     </fill>
   </fills>
@@ -854,7 +859,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -895,6 +900,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1213,8 +1221,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1343,8 +1351,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:V5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="R1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="V5" sqref="V5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1790,10 +1798,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:Q5"/>
+  <dimension ref="A1:R5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="Q1" sqref="Q1:Q1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1806,10 +1814,10 @@
     <col min="8" max="8" width="60" style="3" customWidth="1"/>
     <col min="9" max="10" width="70" style="3" customWidth="1"/>
     <col min="11" max="11" width="35" style="3" customWidth="1"/>
-    <col min="12" max="17" width="60" style="3" customWidth="1"/>
+    <col min="12" max="18" width="60" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>46</v>
       </c>
@@ -1858,11 +1866,14 @@
       <c r="P1" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="Q1" s="7" t="s">
+      <c r="Q1" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="R1" s="7" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>151</v>
       </c>
@@ -1897,7 +1908,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>159</v>
       </c>
@@ -1935,7 +1946,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="127.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" ht="127.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>167</v>
       </c>
@@ -1970,7 +1981,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>176</v>
       </c>

</xml_diff>